<commit_message>
fix mean and std
</commit_message>
<xml_diff>
--- a/analysis/f1-score_analysis.xlsx
+++ b/analysis/f1-score_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lemel\Documents\Université 4\Stage II\uqar\llms4apiclassification\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4180581-F865-4DEB-8239-E2F26B31B3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45D8B27-7615-460D-977D-C443C18579EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15480" xr2:uid="{D13A3AA1-505B-4858-B290-6607CA53DAFD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D13A3AA1-505B-4858-B290-6607CA53DAFD}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="2" r:id="rId1"/>
@@ -156,7 +156,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -349,18 +349,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -374,65 +371,56 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -443,52 +431,55 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -828,7 +819,7 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,1405 +841,1377 @@
       <c r="K1" s="2"/>
     </row>
     <row r="3" spans="3:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="5"/>
-      <c r="O3" s="4" t="s">
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="4"/>
+      <c r="O3" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="P3" s="4"/>
+      <c r="P3" s="49"/>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L4" s="19" t="s">
         <v>24</v>
       </c>
       <c r="N4" s="3"/>
-      <c r="O4" s="33" t="s">
+      <c r="O4" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="18">
+      <c r="P4" s="9">
         <f>AVERAGE(L5:L18)</f>
         <v>73.213016051271936</v>
       </c>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>76.077347384664407</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>83.428966219904694</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>85.318430495548597</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>73.903892337343294</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>74.820029153944802</v>
       </c>
-      <c r="I5" s="42">
+      <c r="I5" s="38">
         <v>85.517597784473907</v>
       </c>
-      <c r="J5" s="10">
-        <f>AVERAGE(D5:I5)</f>
-        <v>79.844377229313281</v>
-      </c>
-      <c r="K5" s="10">
-        <f>_xlfn.STDEV.P(D5:I5)</f>
-        <v>4.9953964981972101</v>
-      </c>
-      <c r="L5" s="23">
+      <c r="J5" s="9">
+        <v>79.844377229313295</v>
+      </c>
+      <c r="K5" s="9">
+        <v>5.4292513704857903</v>
+      </c>
+      <c r="L5" s="20">
         <f>MAX(D5:I5)</f>
         <v>85.517597784473907</v>
       </c>
-      <c r="O5" s="34" t="s">
+      <c r="O5" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="18">
+      <c r="P5" s="9">
         <f>_xlfn.STDEV.P(L5:L18)</f>
         <v>22.349783235706038</v>
       </c>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>49.870691458022698</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>67.713887005875605</v>
       </c>
-      <c r="F6" s="43">
+      <c r="F6" s="39">
         <v>80.5640888148682</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>51.766203699063702</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>74.496358941017505</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <v>77.618373775949294</v>
       </c>
-      <c r="J6" s="10">
-        <f t="shared" ref="J6:J18" si="0">AVERAGE(D6:I6)</f>
-        <v>67.004933949132834</v>
-      </c>
-      <c r="K6" s="10">
-        <f t="shared" ref="K6:K18" si="1">_xlfn.STDEV.P(D6:I6)</f>
-        <v>12.103174610094946</v>
-      </c>
-      <c r="L6" s="18">
-        <f t="shared" ref="L6:L18" si="2">MAX(D6:I6)</f>
+      <c r="J6" s="9">
+        <v>67.004933949132806</v>
+      </c>
+      <c r="K6" s="9">
+        <v>12.1031746100949</v>
+      </c>
+      <c r="L6" s="9">
+        <f t="shared" ref="L6:L18" si="0">MAX(D6:I6)</f>
         <v>80.5640888148682</v>
       </c>
-      <c r="O6" s="34" t="s">
+      <c r="O6" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="9">
         <f>AVERAGE(L5:L12)</f>
         <v>85.049503744486117</v>
       </c>
     </row>
     <row r="7" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>72.906153143151599</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>73.365029349219</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>85.197323991752199</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>72.421449913993101</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="9">
         <v>51.205566878941497</v>
       </c>
-      <c r="I7" s="42">
+      <c r="I7" s="38">
         <v>85.668584103223694</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="9">
+        <v>73.460684563380198</v>
+      </c>
+      <c r="K7" s="9">
+        <v>11.427076347191401</v>
+      </c>
+      <c r="L7" s="9">
         <f t="shared" si="0"/>
-        <v>73.460684563380184</v>
-      </c>
-      <c r="K7" s="10">
-        <f t="shared" si="1"/>
-        <v>11.427076347191385</v>
-      </c>
-      <c r="L7" s="18">
-        <f t="shared" si="2"/>
         <v>85.668584103223694</v>
       </c>
-      <c r="O7" s="34" t="s">
+      <c r="O7" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="35">
+      <c r="P7" s="31">
         <f>_xlfn.STDEV.P(L5:L12)</f>
         <v>2.4269188849367103</v>
       </c>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>78.574371293874194</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>82.303100255410698</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="39">
         <v>85.465647636764103</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <v>61.323954020938601</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="9">
         <v>47.930142164923097</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <v>84.538040618456293</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
+        <v>73.359209331727897</v>
+      </c>
+      <c r="K8" s="9">
+        <v>14.0758096785821</v>
+      </c>
+      <c r="L8" s="9">
         <f t="shared" si="0"/>
-        <v>73.355875998394509</v>
-      </c>
-      <c r="K8" s="10">
-        <f t="shared" si="1"/>
-        <v>13.965481118457832</v>
-      </c>
-      <c r="L8" s="18">
-        <f t="shared" si="2"/>
         <v>85.465647636764103</v>
       </c>
-      <c r="O8" s="34" t="s">
+      <c r="O8" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="P8" s="18">
+      <c r="P8" s="9">
         <f>AVERAGE(L13:L18)</f>
         <v>57.431032460319706</v>
       </c>
     </row>
     <row r="9" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>62.687672379754503</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>55.9809679783775</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="39">
         <v>82.968447209422294</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>52.313537495321597</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="9">
         <v>67.590276895690096</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>75.041964051563198</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="9">
+        <v>66.097144335021497</v>
+      </c>
+      <c r="K9" s="9">
+        <v>10.5737839796421</v>
+      </c>
+      <c r="L9" s="9">
         <f t="shared" si="0"/>
-        <v>66.097144335021525</v>
-      </c>
-      <c r="K9" s="10">
-        <f t="shared" si="1"/>
-        <v>10.573783979642149</v>
-      </c>
-      <c r="L9" s="18">
-        <f t="shared" si="2"/>
         <v>82.968447209422294</v>
       </c>
-      <c r="O9" s="36" t="s">
+      <c r="O9" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="P9" s="14">
+      <c r="P9" s="13">
         <f>_xlfn.STDEV.P(L13:L18)</f>
         <v>26.866380179469502</v>
       </c>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>72.379691433975793</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>84.129149045305297</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="39">
         <v>84.434784225361994</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>62.448038006191602</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="9">
         <v>59.407050301560503</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <v>82.389965034228993</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="9">
+        <v>74.198113007770701</v>
+      </c>
+      <c r="K10" s="9">
+        <v>10.4801189602937</v>
+      </c>
+      <c r="L10" s="9">
         <f t="shared" si="0"/>
-        <v>74.198113007770701</v>
-      </c>
-      <c r="K10" s="10">
-        <f t="shared" si="1"/>
-        <v>10.25238028915785</v>
-      </c>
-      <c r="L10" s="18">
-        <f t="shared" si="2"/>
         <v>84.434784225361994</v>
       </c>
     </row>
     <row r="11" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>71.623865796829904</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>81.864239264773303</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>82.897088326865799</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>70.755812002952695</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="9">
         <v>79.597327200778096</v>
       </c>
-      <c r="I11" s="42">
+      <c r="I11" s="38">
         <v>86.2456998048754</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="9">
+        <v>78.830672066179204</v>
+      </c>
+      <c r="K11" s="9">
+        <v>6.0448287904488804</v>
+      </c>
+      <c r="L11" s="9">
         <f t="shared" si="0"/>
-        <v>78.83067206617919</v>
-      </c>
-      <c r="K11" s="10">
-        <f t="shared" si="1"/>
-        <v>5.7510881471716013</v>
-      </c>
-      <c r="L11" s="18">
-        <f t="shared" si="2"/>
         <v>86.2456998048754</v>
       </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <v>85.706501158796698</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="40">
         <v>89.5311803768993</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="11">
         <v>89.075049484431602</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="11">
         <v>83.441814981991797</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="11">
         <v>89.350230330336899</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="12">
         <v>87.094576668028907</v>
       </c>
-      <c r="J12" s="37">
+      <c r="J12" s="33">
+        <v>87.366558833414203</v>
+      </c>
+      <c r="K12" s="34">
+        <v>3.2241142865407801</v>
+      </c>
+      <c r="L12" s="34">
         <f t="shared" si="0"/>
-        <v>87.366558833414203</v>
-      </c>
-      <c r="K12" s="38">
-        <f t="shared" si="1"/>
-        <v>2.227586863980068</v>
-      </c>
-      <c r="L12" s="38">
-        <f t="shared" si="2"/>
         <v>89.5311803768993</v>
       </c>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>0.38252950285306198</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>0.96982594303256897</v>
       </c>
-      <c r="F13" s="43">
+      <c r="F13" s="39">
         <v>64.127047354602098</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <v>32.313391544379201</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="9">
         <v>47.986932729520397</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="10">
         <v>61.2054137488823</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="9">
+        <v>34.497523470544898</v>
+      </c>
+      <c r="K13" s="9">
+        <v>26.086578273576599</v>
+      </c>
+      <c r="L13" s="9">
         <f t="shared" si="0"/>
-        <v>34.497523470544941</v>
-      </c>
-      <c r="K13" s="10">
-        <f t="shared" si="1"/>
-        <v>26.031692216907011</v>
-      </c>
-      <c r="L13" s="18">
-        <f t="shared" si="2"/>
         <v>64.127047354602098</v>
       </c>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>72.081701296921494</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>82.052702932243704</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="9">
         <v>81.255170741620304</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="9">
         <v>60.847469263802999</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="9">
         <v>13.6397556718434</v>
       </c>
-      <c r="I14" s="42">
+      <c r="I14" s="38">
         <v>84.958475731106901</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="9">
+        <v>65.805879272923093</v>
+      </c>
+      <c r="K14" s="9">
+        <v>24.745096113349099</v>
+      </c>
+      <c r="L14" s="9">
         <f t="shared" si="0"/>
-        <v>65.805879272923121</v>
-      </c>
-      <c r="K14" s="10">
-        <f t="shared" si="1"/>
-        <v>24.680417542559368</v>
-      </c>
-      <c r="L14" s="18">
-        <f t="shared" si="2"/>
         <v>84.958475731106901</v>
       </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>6.7363168563854599</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>3.1741012610577801</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="9">
         <v>73.348094825228401</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="9">
         <v>37.355964082029203</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="9">
         <v>9.2332568617153594</v>
       </c>
-      <c r="I15" s="42">
+      <c r="I15" s="38">
         <v>77.043635108852499</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="9">
+        <v>34.481894832544803</v>
+      </c>
+      <c r="K15" s="9">
+        <v>30.870245291644999</v>
+      </c>
+      <c r="L15" s="9">
         <f t="shared" si="0"/>
-        <v>34.481894832544782</v>
-      </c>
-      <c r="K15" s="10">
-        <f t="shared" si="1"/>
-        <v>30.870245291644988</v>
-      </c>
-      <c r="L15" s="18">
-        <f t="shared" si="2"/>
         <v>77.043635108852499</v>
       </c>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="11">
         <v>0</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="11">
         <v>0</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="11">
         <v>0</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="11">
         <v>3.1188205733660199</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="11">
         <v>0</v>
       </c>
-      <c r="I16" s="45">
+      <c r="I16" s="41">
         <v>6.0964636980814904</v>
       </c>
-      <c r="J16" s="39">
+      <c r="J16" s="35">
+        <v>1.5358807119079201</v>
+      </c>
+      <c r="K16" s="45">
+        <v>2.3359628287429199</v>
+      </c>
+      <c r="L16" s="37">
         <f t="shared" si="0"/>
-        <v>1.5358807119079183</v>
-      </c>
-      <c r="K16" s="50">
-        <f t="shared" si="1"/>
-        <v>2.335962828742927</v>
-      </c>
-      <c r="L16" s="41">
-        <f t="shared" si="2"/>
         <v>6.0964636980814904</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>0</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>0</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <v>2.46731046731046</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="9">
         <v>40.317172587284901</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="9">
         <v>23.603852789045501</v>
       </c>
-      <c r="I17" s="42">
+      <c r="I17" s="38">
         <v>72.073629243816796</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="9">
+        <v>23.076994181242899</v>
+      </c>
+      <c r="K17" s="37">
+        <v>26.467395933395998</v>
+      </c>
+      <c r="L17" s="20">
         <f t="shared" si="0"/>
-        <v>23.076994181242942</v>
-      </c>
-      <c r="K17" s="41">
-        <f t="shared" si="1"/>
-        <v>26.419771518663783</v>
-      </c>
-      <c r="L17" s="23">
-        <f t="shared" si="2"/>
         <v>72.073629243816796</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="13">
         <v>0</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <v>0</v>
       </c>
-      <c r="F18" s="46">
+      <c r="F18" s="42">
         <v>40.286943625458498</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <v>0.165289256198347</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="13">
         <v>0.31861471861471802</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="14">
         <v>23.716781628940002</v>
       </c>
-      <c r="J18" s="32">
+      <c r="J18" s="29">
+        <v>10.7479382048686</v>
+      </c>
+      <c r="K18" s="13">
+        <v>15.8156744442941</v>
+      </c>
+      <c r="L18" s="13">
         <f t="shared" si="0"/>
-        <v>10.747938204868595</v>
-      </c>
-      <c r="K18" s="14">
-        <f t="shared" si="1"/>
-        <v>15.772039286126923</v>
-      </c>
-      <c r="L18" s="14">
-        <f t="shared" si="2"/>
         <v>40.286943625458498</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="9">
         <f>MIN(D5:D18)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="18">
-        <f t="shared" ref="E19:I19" si="3">MIN(E5:E18)</f>
+      <c r="E19" s="9">
+        <f t="shared" ref="E19:I19" si="1">MIN(E5:E18)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="18">
-        <f t="shared" si="3"/>
+      <c r="F19" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G19" s="18">
-        <f t="shared" si="3"/>
+      <c r="G19" s="9">
+        <f t="shared" si="1"/>
         <v>0.165289256198347</v>
       </c>
-      <c r="H19" s="18">
-        <f t="shared" si="3"/>
+      <c r="H19" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I19" s="19">
-        <f t="shared" si="3"/>
+      <c r="I19" s="17">
+        <f t="shared" si="1"/>
         <v>6.0964636980814904</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="9">
         <f>MAX(D5:D18)</f>
         <v>85.706501158796698</v>
       </c>
-      <c r="E20" s="18">
-        <f t="shared" ref="E20:I20" si="4">MAX(E5:E18)</f>
+      <c r="E20" s="9">
+        <f t="shared" ref="E20:I20" si="2">MAX(E5:E18)</f>
         <v>89.5311803768993</v>
       </c>
-      <c r="F20" s="18">
-        <f t="shared" si="4"/>
+      <c r="F20" s="9">
+        <f t="shared" si="2"/>
         <v>89.075049484431602</v>
       </c>
-      <c r="G20" s="18">
-        <f t="shared" si="4"/>
+      <c r="G20" s="9">
+        <f t="shared" si="2"/>
         <v>83.441814981991797</v>
       </c>
-      <c r="H20" s="18">
-        <f t="shared" si="4"/>
+      <c r="H20" s="9">
+        <f t="shared" si="2"/>
         <v>89.350230330336899</v>
       </c>
-      <c r="I20" s="11">
-        <f t="shared" si="4"/>
+      <c r="I20" s="10">
+        <f t="shared" si="2"/>
         <v>87.094576668028907</v>
       </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="13">
         <f>D20-D19</f>
         <v>85.706501158796698</v>
       </c>
-      <c r="E21" s="14">
-        <f t="shared" ref="E21:I21" si="5">E20-E19</f>
+      <c r="E21" s="13">
+        <f t="shared" ref="E21:I21" si="3">E20-E19</f>
         <v>89.5311803768993</v>
       </c>
-      <c r="F21" s="14">
-        <f t="shared" si="5"/>
+      <c r="F21" s="13">
+        <f t="shared" si="3"/>
         <v>89.075049484431602</v>
       </c>
-      <c r="G21" s="14">
-        <f t="shared" si="5"/>
+      <c r="G21" s="13">
+        <f t="shared" si="3"/>
         <v>83.276525725793448</v>
       </c>
-      <c r="H21" s="14">
-        <f t="shared" si="5"/>
+      <c r="H21" s="13">
+        <f t="shared" si="3"/>
         <v>89.350230330336899</v>
       </c>
-      <c r="I21" s="15">
-        <f t="shared" si="5"/>
+      <c r="I21" s="14">
+        <f t="shared" si="3"/>
         <v>80.998112969947414</v>
       </c>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
     </row>
     <row r="26" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8" t="s">
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="J27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K27" s="8" t="s">
+      <c r="K27" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L27" s="8" t="s">
+      <c r="L27" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="18">
-        <f>E5-$D5</f>
+      <c r="D28" s="15"/>
+      <c r="E28" s="9">
+        <f t="shared" ref="E28:I41" si="4">E5-$D5</f>
         <v>7.3516188352402878</v>
       </c>
-      <c r="F28" s="18">
-        <f>F5-$D5</f>
+      <c r="F28" s="9">
+        <f t="shared" si="4"/>
         <v>9.2410831108841904</v>
       </c>
-      <c r="G28" s="18">
-        <f>G5-$D5</f>
+      <c r="G28" s="9">
+        <f t="shared" si="4"/>
         <v>-2.1734550473211129</v>
       </c>
-      <c r="H28" s="18">
-        <f>H5-$D5</f>
+      <c r="H28" s="9">
+        <f t="shared" si="4"/>
         <v>-1.2573182307196049</v>
       </c>
-      <c r="I28" s="11">
-        <f>I5-$D5</f>
+      <c r="I28" s="10">
+        <f t="shared" si="4"/>
         <v>9.4402503998095</v>
       </c>
-      <c r="J28" s="18">
+      <c r="J28" s="9">
         <f>MIN(E28:I28)</f>
         <v>-2.1734550473211129</v>
       </c>
-      <c r="K28" s="18">
+      <c r="K28" s="9">
         <f>MAX(E28:J28)</f>
         <v>9.4402503998095</v>
       </c>
-      <c r="L28" s="18">
+      <c r="L28" s="9">
         <f>K28-J28</f>
         <v>11.613705447130613</v>
       </c>
-      <c r="N28" s="52" t="s">
+      <c r="N28" s="47" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="18">
-        <f>E6-$D6</f>
+      <c r="D29" s="15"/>
+      <c r="E29" s="9">
+        <f t="shared" si="4"/>
         <v>17.843195547852908</v>
       </c>
-      <c r="F29" s="18">
-        <f>F6-$D6</f>
+      <c r="F29" s="9">
+        <f t="shared" si="4"/>
         <v>30.693397356845502</v>
       </c>
-      <c r="G29" s="18">
-        <f>G6-$D6</f>
+      <c r="G29" s="9">
+        <f t="shared" si="4"/>
         <v>1.8955122410410041</v>
       </c>
-      <c r="H29" s="18">
-        <f>H6-$D6</f>
+      <c r="H29" s="9">
+        <f t="shared" si="4"/>
         <v>24.625667482994807</v>
       </c>
-      <c r="I29" s="11">
-        <f>I6-$D6</f>
+      <c r="I29" s="10">
+        <f t="shared" si="4"/>
         <v>27.747682317926596</v>
       </c>
-      <c r="J29" s="48">
-        <f t="shared" ref="J29:J41" si="6">MIN(E29:I29)</f>
+      <c r="J29" s="43">
+        <f t="shared" ref="J29:J41" si="5">MIN(E29:I29)</f>
         <v>1.8955122410410041</v>
       </c>
-      <c r="K29" s="18">
-        <f t="shared" ref="K29:K41" si="7">MAX(E29:J29)</f>
+      <c r="K29" s="9">
+        <f t="shared" ref="K29:K41" si="6">MAX(E29:J29)</f>
         <v>30.693397356845502</v>
       </c>
-      <c r="L29" s="18">
-        <f t="shared" ref="L29:L41" si="8">K29-J29</f>
+      <c r="L29" s="9">
+        <f t="shared" ref="L29:L41" si="7">K29-J29</f>
         <v>28.797885115804498</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="18">
-        <f>E7-$D7</f>
+      <c r="D30" s="15"/>
+      <c r="E30" s="9">
+        <f t="shared" si="4"/>
         <v>0.45887620606740143</v>
       </c>
-      <c r="F30" s="18">
-        <f>F7-$D7</f>
+      <c r="F30" s="9">
+        <f t="shared" si="4"/>
         <v>12.291170848600601</v>
       </c>
-      <c r="G30" s="18">
-        <f>G7-$D7</f>
+      <c r="G30" s="9">
+        <f t="shared" si="4"/>
         <v>-0.48470322915849806</v>
       </c>
-      <c r="H30" s="18">
-        <f>H7-$D7</f>
+      <c r="H30" s="9">
+        <f t="shared" si="4"/>
         <v>-21.700586264210102</v>
       </c>
-      <c r="I30" s="11">
-        <f>I7-$D7</f>
+      <c r="I30" s="10">
+        <f t="shared" si="4"/>
         <v>12.762430960072095</v>
       </c>
-      <c r="J30" s="18">
+      <c r="J30" s="9">
+        <f t="shared" si="5"/>
+        <v>-21.700586264210102</v>
+      </c>
+      <c r="K30" s="9">
         <f t="shared" si="6"/>
-        <v>-21.700586264210102</v>
-      </c>
-      <c r="K30" s="18">
+        <v>12.762430960072095</v>
+      </c>
+      <c r="L30" s="44">
         <f t="shared" si="7"/>
-        <v>12.762430960072095</v>
-      </c>
-      <c r="L30" s="49">
-        <f t="shared" si="8"/>
         <v>34.463017224282197</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="18">
-        <f>E8-$D8</f>
+      <c r="D31" s="15"/>
+      <c r="E31" s="9">
+        <f t="shared" si="4"/>
         <v>3.728728961536504</v>
       </c>
-      <c r="F31" s="18">
-        <f>F8-$D8</f>
+      <c r="F31" s="9">
+        <f t="shared" si="4"/>
         <v>6.8912763428899098</v>
       </c>
-      <c r="G31" s="18">
-        <f>G8-$D8</f>
+      <c r="G31" s="9">
+        <f t="shared" si="4"/>
         <v>-17.250417272935593</v>
       </c>
-      <c r="H31" s="18">
-        <f>H8-$D8</f>
+      <c r="H31" s="9">
+        <f t="shared" si="4"/>
         <v>-30.644229128951096</v>
       </c>
-      <c r="I31" s="11">
-        <f>I8-$D8</f>
+      <c r="I31" s="10">
+        <f t="shared" si="4"/>
         <v>5.9636693245820993</v>
       </c>
-      <c r="J31" s="18">
+      <c r="J31" s="9">
+        <f t="shared" si="5"/>
+        <v>-30.644229128951096</v>
+      </c>
+      <c r="K31" s="9">
         <f t="shared" si="6"/>
-        <v>-30.644229128951096</v>
-      </c>
-      <c r="K31" s="18">
+        <v>6.8912763428899098</v>
+      </c>
+      <c r="L31" s="44">
         <f t="shared" si="7"/>
-        <v>6.8912763428899098</v>
-      </c>
-      <c r="L31" s="49">
-        <f t="shared" si="8"/>
         <v>37.535505471841006</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="18">
-        <f>E9-$D9</f>
+      <c r="D32" s="15"/>
+      <c r="E32" s="9">
+        <f t="shared" si="4"/>
         <v>-6.706704401377003</v>
       </c>
-      <c r="F32" s="18">
-        <f>F9-$D9</f>
+      <c r="F32" s="9">
+        <f t="shared" si="4"/>
         <v>20.280774829667791</v>
       </c>
-      <c r="G32" s="18">
-        <f>G9-$D9</f>
+      <c r="G32" s="9">
+        <f t="shared" si="4"/>
         <v>-10.374134884432905</v>
       </c>
-      <c r="H32" s="18">
-        <f>H9-$D9</f>
+      <c r="H32" s="9">
+        <f t="shared" si="4"/>
         <v>4.9026045159355931</v>
       </c>
-      <c r="I32" s="11">
-        <f>I9-$D9</f>
+      <c r="I32" s="10">
+        <f t="shared" si="4"/>
         <v>12.354291671808696</v>
       </c>
-      <c r="J32" s="18">
+      <c r="J32" s="9">
+        <f t="shared" si="5"/>
+        <v>-10.374134884432905</v>
+      </c>
+      <c r="K32" s="9">
         <f t="shared" si="6"/>
-        <v>-10.374134884432905</v>
-      </c>
-      <c r="K32" s="18">
+        <v>20.280774829667791</v>
+      </c>
+      <c r="L32" s="44">
         <f t="shared" si="7"/>
-        <v>20.280774829667791</v>
-      </c>
-      <c r="L32" s="49">
-        <f t="shared" si="8"/>
         <v>30.654909714100697</v>
       </c>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="18">
-        <f>E10-$D10</f>
+      <c r="D33" s="15"/>
+      <c r="E33" s="9">
+        <f t="shared" si="4"/>
         <v>11.749457611329504</v>
       </c>
-      <c r="F33" s="18">
-        <f>F10-$D10</f>
+      <c r="F33" s="9">
+        <f t="shared" si="4"/>
         <v>12.055092791386201</v>
       </c>
-      <c r="G33" s="18">
-        <f>G10-$D10</f>
+      <c r="G33" s="9">
+        <f t="shared" si="4"/>
         <v>-9.931653427784191</v>
       </c>
-      <c r="H33" s="18">
-        <f>H10-$D10</f>
+      <c r="H33" s="9">
+        <f t="shared" si="4"/>
         <v>-12.972641132415291</v>
       </c>
-      <c r="I33" s="11">
-        <f>I10-$D10</f>
+      <c r="I33" s="10">
+        <f t="shared" si="4"/>
         <v>10.0102736002532</v>
       </c>
-      <c r="J33" s="18">
+      <c r="J33" s="9">
+        <f t="shared" si="5"/>
+        <v>-12.972641132415291</v>
+      </c>
+      <c r="K33" s="9">
         <f t="shared" si="6"/>
-        <v>-12.972641132415291</v>
-      </c>
-      <c r="K33" s="18">
+        <v>12.055092791386201</v>
+      </c>
+      <c r="L33" s="9">
         <f t="shared" si="7"/>
-        <v>12.055092791386201</v>
-      </c>
-      <c r="L33" s="18">
-        <f t="shared" si="8"/>
         <v>25.027733923801492</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="18">
-        <f>E11-$D11</f>
+      <c r="D34" s="15"/>
+      <c r="E34" s="9">
+        <f t="shared" si="4"/>
         <v>10.2403734679434</v>
       </c>
-      <c r="F34" s="18">
-        <f>F11-$D11</f>
+      <c r="F34" s="9">
+        <f t="shared" si="4"/>
         <v>11.273222530035895</v>
       </c>
-      <c r="G34" s="18">
-        <f>G11-$D11</f>
+      <c r="G34" s="9">
+        <f t="shared" si="4"/>
         <v>-0.86805379387720905</v>
       </c>
-      <c r="H34" s="18">
-        <f>H11-$D11</f>
+      <c r="H34" s="9">
+        <f t="shared" si="4"/>
         <v>7.9734614039481926</v>
       </c>
-      <c r="I34" s="11">
-        <f>I11-$D11</f>
+      <c r="I34" s="10">
+        <f t="shared" si="4"/>
         <v>14.621834008045496</v>
       </c>
-      <c r="J34" s="18">
+      <c r="J34" s="9">
+        <f t="shared" si="5"/>
+        <v>-0.86805379387720905</v>
+      </c>
+      <c r="K34" s="9">
         <f t="shared" si="6"/>
-        <v>-0.86805379387720905</v>
-      </c>
-      <c r="K34" s="18">
+        <v>14.621834008045496</v>
+      </c>
+      <c r="L34" s="9">
         <f t="shared" si="7"/>
-        <v>14.621834008045496</v>
-      </c>
-      <c r="L34" s="18">
-        <f t="shared" si="8"/>
         <v>15.489887801922706</v>
       </c>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="24"/>
-      <c r="E35" s="12">
-        <f>E12-$D12</f>
+      <c r="D35" s="21"/>
+      <c r="E35" s="11">
+        <f t="shared" si="4"/>
         <v>3.8246792181026024</v>
       </c>
-      <c r="F35" s="12">
-        <f>F12-$D12</f>
+      <c r="F35" s="11">
+        <f t="shared" si="4"/>
         <v>3.3685483256349045</v>
       </c>
-      <c r="G35" s="12">
-        <f>G12-$D12</f>
+      <c r="G35" s="11">
+        <f t="shared" si="4"/>
         <v>-2.2646861768049007</v>
       </c>
-      <c r="H35" s="12">
-        <f>H12-$D12</f>
+      <c r="H35" s="11">
+        <f t="shared" si="4"/>
         <v>3.6437291715402012</v>
       </c>
-      <c r="I35" s="13">
-        <f>I12-$D12</f>
+      <c r="I35" s="12">
+        <f t="shared" si="4"/>
         <v>1.388075509232209</v>
       </c>
-      <c r="J35" s="12">
+      <c r="J35" s="11">
+        <f t="shared" si="5"/>
+        <v>-2.2646861768049007</v>
+      </c>
+      <c r="K35" s="36">
         <f t="shared" si="6"/>
-        <v>-2.2646861768049007</v>
-      </c>
-      <c r="K35" s="40">
+        <v>3.8246792181026024</v>
+      </c>
+      <c r="L35" s="11">
         <f t="shared" si="7"/>
-        <v>3.8246792181026024</v>
-      </c>
-      <c r="L35" s="12">
-        <f t="shared" si="8"/>
         <v>6.0893653949075031</v>
       </c>
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="18">
-        <f>E13-$D13</f>
+      <c r="D36" s="15"/>
+      <c r="E36" s="9">
+        <f t="shared" si="4"/>
         <v>0.587296440179507</v>
       </c>
-      <c r="F36" s="18">
-        <f>F13-$D13</f>
+      <c r="F36" s="9">
+        <f t="shared" si="4"/>
         <v>63.744517851749038</v>
       </c>
-      <c r="G36" s="18">
-        <f>G13-$D13</f>
+      <c r="G36" s="9">
+        <f t="shared" si="4"/>
         <v>31.93086204152614</v>
       </c>
-      <c r="H36" s="18">
-        <f>H13-$D13</f>
+      <c r="H36" s="9">
+        <f t="shared" si="4"/>
         <v>47.604403226667337</v>
       </c>
-      <c r="I36" s="11">
-        <f>I13-$D13</f>
+      <c r="I36" s="10">
+        <f t="shared" si="4"/>
         <v>60.82288424602924</v>
       </c>
-      <c r="J36" s="18">
+      <c r="J36" s="9">
+        <f t="shared" si="5"/>
+        <v>0.587296440179507</v>
+      </c>
+      <c r="K36" s="9">
         <f t="shared" si="6"/>
-        <v>0.587296440179507</v>
-      </c>
-      <c r="K36" s="18">
+        <v>63.744517851749038</v>
+      </c>
+      <c r="L36" s="44">
         <f t="shared" si="7"/>
-        <v>63.744517851749038</v>
-      </c>
-      <c r="L36" s="49">
-        <f t="shared" si="8"/>
         <v>63.15722141156953</v>
       </c>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="18">
-        <f>E14-$D14</f>
+      <c r="D37" s="15"/>
+      <c r="E37" s="9">
+        <f t="shared" si="4"/>
         <v>9.9710016353222102</v>
       </c>
-      <c r="F37" s="18">
-        <f>F14-$D14</f>
+      <c r="F37" s="9">
+        <f t="shared" si="4"/>
         <v>9.1734694446988101</v>
       </c>
-      <c r="G37" s="18">
-        <f>G14-$D14</f>
+      <c r="G37" s="9">
+        <f t="shared" si="4"/>
         <v>-11.234232033118495</v>
       </c>
-      <c r="H37" s="18">
-        <f>H14-$D14</f>
+      <c r="H37" s="9">
+        <f t="shared" si="4"/>
         <v>-58.441945625078091</v>
       </c>
-      <c r="I37" s="11">
-        <f>I14-$D14</f>
+      <c r="I37" s="10">
+        <f t="shared" si="4"/>
         <v>12.876774434185407</v>
       </c>
-      <c r="J37" s="47">
+      <c r="J37" s="37">
+        <f t="shared" si="5"/>
+        <v>-58.441945625078091</v>
+      </c>
+      <c r="K37" s="9">
         <f t="shared" si="6"/>
-        <v>-58.441945625078091</v>
-      </c>
-      <c r="K37" s="18">
+        <v>12.876774434185407</v>
+      </c>
+      <c r="L37" s="44">
         <f t="shared" si="7"/>
-        <v>12.876774434185407</v>
-      </c>
-      <c r="L37" s="49">
-        <f t="shared" si="8"/>
         <v>71.318720059263498</v>
       </c>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="16"/>
-      <c r="E38" s="18">
-        <f>E15-$D15</f>
+      <c r="D38" s="15"/>
+      <c r="E38" s="9">
+        <f t="shared" si="4"/>
         <v>-3.5622155953276797</v>
       </c>
-      <c r="F38" s="18">
-        <f>F15-$D15</f>
+      <c r="F38" s="9">
+        <f t="shared" si="4"/>
         <v>66.611777968842944</v>
       </c>
-      <c r="G38" s="18">
-        <f>G15-$D15</f>
+      <c r="G38" s="9">
+        <f t="shared" si="4"/>
         <v>30.619647225643742</v>
       </c>
-      <c r="H38" s="18">
-        <f>H15-$D15</f>
+      <c r="H38" s="9">
+        <f t="shared" si="4"/>
         <v>2.4969400053298996</v>
       </c>
-      <c r="I38" s="11">
-        <f>I15-$D15</f>
+      <c r="I38" s="10">
+        <f t="shared" si="4"/>
         <v>70.307318252467041</v>
       </c>
-      <c r="J38" s="18">
+      <c r="J38" s="9">
+        <f t="shared" si="5"/>
+        <v>-3.5622155953276797</v>
+      </c>
+      <c r="K38" s="9">
         <f t="shared" si="6"/>
-        <v>-3.5622155953276797</v>
-      </c>
-      <c r="K38" s="18">
+        <v>70.307318252467041</v>
+      </c>
+      <c r="L38" s="44">
         <f t="shared" si="7"/>
-        <v>70.307318252467041</v>
-      </c>
-      <c r="L38" s="49">
-        <f t="shared" si="8"/>
         <v>73.869533847794727</v>
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="24"/>
-      <c r="E39" s="12">
-        <f>E16-$D16</f>
+      <c r="D39" s="21"/>
+      <c r="E39" s="11">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F39" s="12">
-        <f>F16-$D16</f>
+      <c r="F39" s="11">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G39" s="12">
-        <f>G16-$D16</f>
+      <c r="G39" s="11">
+        <f t="shared" si="4"/>
         <v>3.1188205733660199</v>
       </c>
-      <c r="H39" s="12">
-        <f>H16-$D16</f>
+      <c r="H39" s="11">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I39" s="13">
-        <f>I16-$D16</f>
+      <c r="I39" s="12">
+        <f t="shared" si="4"/>
         <v>6.0964636980814904</v>
       </c>
-      <c r="J39" s="12">
+      <c r="J39" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K39" s="11">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K39" s="12">
+        <v>6.0964636980814904</v>
+      </c>
+      <c r="L39" s="11">
         <f t="shared" si="7"/>
         <v>6.0964636980814904</v>
       </c>
-      <c r="L39" s="12">
-        <f t="shared" si="8"/>
-        <v>6.0964636980814904</v>
-      </c>
     </row>
     <row r="40" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="18">
-        <f>E17-$D17</f>
+      <c r="D40" s="15"/>
+      <c r="E40" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F40" s="18">
-        <f>F17-$D17</f>
+      <c r="F40" s="9">
+        <f t="shared" si="4"/>
         <v>2.46731046731046</v>
       </c>
-      <c r="G40" s="18">
-        <f>G17-$D17</f>
+      <c r="G40" s="9">
+        <f t="shared" si="4"/>
         <v>40.317172587284901</v>
       </c>
-      <c r="H40" s="18">
-        <f>H17-$D17</f>
+      <c r="H40" s="9">
+        <f t="shared" si="4"/>
         <v>23.603852789045501</v>
       </c>
-      <c r="I40" s="11">
-        <f>I17-$D17</f>
+      <c r="I40" s="10">
+        <f t="shared" si="4"/>
         <v>72.073629243816796</v>
       </c>
-      <c r="J40" s="18">
+      <c r="J40" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K40" s="43">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K40" s="48">
+        <v>72.073629243816796</v>
+      </c>
+      <c r="L40" s="44">
         <f t="shared" si="7"/>
         <v>72.073629243816796</v>
       </c>
-      <c r="L40" s="49">
-        <f t="shared" si="8"/>
-        <v>72.073629243816796</v>
-      </c>
     </row>
     <row r="41" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="27" t="s">
+      <c r="C41" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="14">
-        <f>E18-$D18</f>
+      <c r="D41" s="16"/>
+      <c r="E41" s="13">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F41" s="14">
-        <f>F18-$D18</f>
+      <c r="F41" s="13">
+        <f t="shared" si="4"/>
         <v>40.286943625458498</v>
       </c>
-      <c r="G41" s="14">
-        <f>G18-$D18</f>
+      <c r="G41" s="13">
+        <f t="shared" si="4"/>
         <v>0.165289256198347</v>
       </c>
-      <c r="H41" s="14">
-        <f>H18-$D18</f>
+      <c r="H41" s="13">
+        <f t="shared" si="4"/>
         <v>0.31861471861471802</v>
       </c>
-      <c r="I41" s="15">
-        <f>I18-$D18</f>
+      <c r="I41" s="14">
+        <f t="shared" si="4"/>
         <v>23.716781628940002</v>
       </c>
-      <c r="J41" s="14">
+      <c r="J41" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K41" s="13">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K41" s="14">
+        <v>40.286943625458498</v>
+      </c>
+      <c r="L41" s="46">
         <f t="shared" si="7"/>
         <v>40.286943625458498</v>
       </c>
-      <c r="L41" s="51">
-        <f t="shared" si="8"/>
-        <v>40.286943625458498</v>
-      </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="16"/>
-      <c r="E42" s="18">
+      <c r="D42" s="15"/>
+      <c r="E42" s="9">
         <f>MIN(E28:E41)</f>
         <v>-6.706704401377003</v>
       </c>
-      <c r="F42" s="18">
-        <f t="shared" ref="F42:I42" si="9">MIN(F28:F41)</f>
+      <c r="F42" s="9">
+        <f t="shared" ref="F42:I42" si="8">MIN(F28:F41)</f>
         <v>0</v>
       </c>
-      <c r="G42" s="18">
-        <f t="shared" si="9"/>
+      <c r="G42" s="9">
+        <f t="shared" si="8"/>
         <v>-17.250417272935593</v>
       </c>
-      <c r="H42" s="18">
-        <f t="shared" si="9"/>
+      <c r="H42" s="9">
+        <f t="shared" si="8"/>
         <v>-58.441945625078091</v>
       </c>
-      <c r="I42" s="11">
-        <f t="shared" si="9"/>
+      <c r="I42" s="10">
+        <f t="shared" si="8"/>
         <v>1.388075509232209</v>
       </c>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C43" s="25" t="s">
+      <c r="C43" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="16"/>
-      <c r="E43" s="18">
+      <c r="D43" s="15"/>
+      <c r="E43" s="9">
         <f>MAX(E28:E41)</f>
         <v>17.843195547852908</v>
       </c>
-      <c r="F43" s="18">
-        <f t="shared" ref="F43:I43" si="10">MAX(F28:F41)</f>
+      <c r="F43" s="9">
+        <f t="shared" ref="F43:I43" si="9">MAX(F28:F41)</f>
         <v>66.611777968842944</v>
       </c>
-      <c r="G43" s="18">
-        <f t="shared" si="10"/>
+      <c r="G43" s="9">
+        <f t="shared" si="9"/>
         <v>40.317172587284901</v>
       </c>
-      <c r="H43" s="18">
-        <f t="shared" si="10"/>
+      <c r="H43" s="9">
+        <f t="shared" si="9"/>
         <v>47.604403226667337</v>
       </c>
-      <c r="I43" s="11">
-        <f t="shared" si="10"/>
+      <c r="I43" s="10">
+        <f t="shared" si="9"/>
         <v>72.073629243816796</v>
       </c>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D44" s="16"/>
-      <c r="E44" s="18">
+      <c r="D44" s="15"/>
+      <c r="E44" s="9">
         <f>E43-E42</f>
         <v>24.549899949229911</v>
       </c>
-      <c r="F44" s="18">
-        <f t="shared" ref="F44:I44" si="11">F43-F42</f>
+      <c r="F44" s="9">
+        <f t="shared" ref="F44:I44" si="10">F43-F42</f>
         <v>66.611777968842944</v>
       </c>
-      <c r="G44" s="18">
-        <f t="shared" si="11"/>
+      <c r="G44" s="9">
+        <f t="shared" si="10"/>
         <v>57.567589860220494</v>
       </c>
-      <c r="H44" s="18">
-        <f t="shared" si="11"/>
+      <c r="H44" s="9">
+        <f t="shared" si="10"/>
         <v>106.04634885174542</v>
       </c>
-      <c r="I44" s="11">
-        <f t="shared" si="11"/>
+      <c r="I44" s="10">
+        <f t="shared" si="10"/>
         <v>70.685553734584587</v>
       </c>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="16"/>
-      <c r="E45" s="18">
+      <c r="D45" s="15"/>
+      <c r="E45" s="9">
         <f>AVERAGE(E28:E41)</f>
         <v>3.9633077090621174</v>
       </c>
-      <c r="F45" s="18">
-        <f t="shared" ref="F45:I45" si="12">AVERAGE(F28:F41)</f>
+      <c r="F45" s="9">
+        <f t="shared" ref="F45:I45" si="11">AVERAGE(F28:F41)</f>
         <v>20.598470392428911</v>
       </c>
-      <c r="G45" s="18">
-        <f t="shared" si="12"/>
+      <c r="G45" s="9">
+        <f t="shared" si="11"/>
         <v>3.8189977185448036</v>
       </c>
-      <c r="H45" s="18">
-        <f t="shared" si="12"/>
+      <c r="H45" s="9">
+        <f t="shared" si="11"/>
         <v>-0.70338907623556701</v>
       </c>
-      <c r="I45" s="11">
-        <f t="shared" si="12"/>
+      <c r="I45" s="10">
+        <f t="shared" si="11"/>
         <v>24.298739949660707</v>
       </c>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
     </row>
     <row r="46" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="27" t="s">
+      <c r="C46" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="14">
+      <c r="D46" s="16"/>
+      <c r="E46" s="13">
         <f>_xlfn.STDEV.P(E28:E41)</f>
         <v>6.4454237951365903</v>
       </c>
-      <c r="F46" s="14">
-        <f t="shared" ref="F46:I46" si="13">_xlfn.STDEV.P(F28:F41)</f>
+      <c r="F46" s="13">
+        <f t="shared" ref="F46:I46" si="12">_xlfn.STDEV.P(F28:F41)</f>
         <v>21.035217641671611</v>
       </c>
-      <c r="G46" s="14">
-        <f t="shared" si="13"/>
+      <c r="G46" s="13">
+        <f t="shared" si="12"/>
         <v>16.971961154672947</v>
       </c>
-      <c r="H46" s="14">
-        <f t="shared" si="13"/>
+      <c r="H46" s="13">
+        <f t="shared" si="12"/>
         <v>24.676996356919908</v>
       </c>
-      <c r="I46" s="15">
-        <f t="shared" si="13"/>
+      <c r="I46" s="14">
+        <f t="shared" si="12"/>
         <v>23.69850447004832</v>
       </c>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
update excel tables with new models
</commit_message>
<xml_diff>
--- a/analysis/f1-score_analysis.xlsx
+++ b/analysis/f1-score_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lemel\Documents\Université 4\Stage II\uqar\llms4apiclassification\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45D8B27-7615-460D-977D-C443C18579EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC2A89E-FFE2-46DF-8750-289B9F1DAF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D13A3AA1-505B-4858-B290-6607CA53DAFD}"/>
+    <workbookView xWindow="15156" yWindow="-13800" windowWidth="21144" windowHeight="12696" xr2:uid="{D13A3AA1-505B-4858-B290-6607CA53DAFD}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="2" r:id="rId1"/>
@@ -85,24 +85,12 @@
     <t>Mistral–Large–2</t>
   </si>
   <si>
-    <t>Qwen2</t>
-  </si>
-  <si>
-    <t>Phi–3</t>
-  </si>
-  <si>
-    <t>DeepSeek–V2</t>
-  </si>
-  <si>
     <t>GPT–4o–Mini</t>
   </si>
   <si>
     <t>Gemini–1.5–Flash</t>
   </si>
   <si>
-    <t xml:space="preserve">CodeQwen1.5 </t>
-  </si>
-  <si>
     <t>DeepSeek–Coder–V2</t>
   </si>
   <si>
@@ -149,6 +137,18 @@
   </si>
   <si>
     <t>&gt; 30</t>
+  </si>
+  <si>
+    <t>Qwen2.5</t>
+  </si>
+  <si>
+    <t>Phi–3.5-MoE</t>
+  </si>
+  <si>
+    <t>DeepSeek–V2.5</t>
+  </si>
+  <si>
+    <t>Qwen2.5-Coder</t>
   </si>
 </sst>
 </file>
@@ -349,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -405,7 +405,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -467,9 +466,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -480,6 +476,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -819,46 +824,46 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="20.5546875" customWidth="1"/>
+    <col min="15" max="15" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:16" x14ac:dyDescent="0.3">
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="3" spans="3:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
+    <row r="3" spans="3:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
       <c r="L3" s="4"/>
-      <c r="O3" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" s="49"/>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="O3" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="47"/>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C4" s="6"/>
       <c r="D4" s="7" t="s">
         <v>0</v>
@@ -885,19 +890,19 @@
         <v>7</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="N4" s="3"/>
-      <c r="O4" s="30" t="s">
-        <v>27</v>
+      <c r="O4" s="29" t="s">
+        <v>23</v>
       </c>
       <c r="P4" s="9">
         <f>AVERAGE(L5:L18)</f>
-        <v>73.213016051271936</v>
-      </c>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="25" t="s">
+        <v>74.214903810221003</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C5" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="9">
@@ -915,7 +920,7 @@
       <c r="H5" s="9">
         <v>74.820029153944802</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="37">
         <v>85.517597784473907</v>
       </c>
       <c r="J5" s="9">
@@ -928,16 +933,16 @@
         <f>MAX(D5:I5)</f>
         <v>85.517597784473907</v>
       </c>
-      <c r="O5" s="30" t="s">
-        <v>28</v>
+      <c r="O5" s="29" t="s">
+        <v>24</v>
       </c>
       <c r="P5" s="9">
         <f>_xlfn.STDEV.P(L5:L18)</f>
-        <v>22.349783235706038</v>
-      </c>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C6" s="25" t="s">
+        <v>22.321578748823072</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C6" s="24" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="9">
@@ -946,7 +951,7 @@
       <c r="E6" s="9">
         <v>67.713887005875605</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="38">
         <v>80.5640888148682</v>
       </c>
       <c r="G6" s="9">
@@ -968,16 +973,16 @@
         <f t="shared" ref="L6:L18" si="0">MAX(D6:I6)</f>
         <v>80.5640888148682</v>
       </c>
-      <c r="O6" s="30" t="s">
-        <v>29</v>
+      <c r="O6" s="29" t="s">
+        <v>25</v>
       </c>
       <c r="P6" s="9">
         <f>AVERAGE(L5:L12)</f>
-        <v>85.049503744486117</v>
-      </c>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C7" s="25" t="s">
+        <v>84.625125914790999</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C7" s="24" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="9">
@@ -995,7 +1000,7 @@
       <c r="H7" s="9">
         <v>51.205566878941497</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="37">
         <v>85.668584103223694</v>
       </c>
       <c r="J7" s="9">
@@ -1008,130 +1013,130 @@
         <f t="shared" si="0"/>
         <v>85.668584103223694</v>
       </c>
-      <c r="O7" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" s="31">
+      <c r="O7" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="30">
         <f>_xlfn.STDEV.P(L5:L12)</f>
-        <v>2.4269188849367103</v>
-      </c>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="25" t="s">
-        <v>13</v>
+        <v>4.1160873726225864</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C8" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="D8" s="9">
-        <v>78.574371293874194</v>
-      </c>
-      <c r="E8" s="9">
-        <v>82.303100255410698</v>
-      </c>
-      <c r="F8" s="39">
-        <v>85.465647636764103</v>
+        <v>75.923487071692406</v>
+      </c>
+      <c r="E8" s="48">
+        <v>86.040156752479803</v>
+      </c>
+      <c r="F8" s="48">
+        <v>85.821885287475496</v>
       </c>
       <c r="G8" s="9">
-        <v>61.323954020938601</v>
-      </c>
-      <c r="H8" s="9">
-        <v>47.930142164923097</v>
+        <v>78.710816662280493</v>
+      </c>
+      <c r="H8" s="38">
+        <v>86.956808148753694</v>
       </c>
       <c r="I8" s="10">
-        <v>84.538040618456293</v>
+        <v>85.546383356422396</v>
       </c>
       <c r="J8" s="9">
-        <v>73.359209331727897</v>
+        <v>83.1665895465174</v>
       </c>
       <c r="K8" s="9">
-        <v>14.0758096785821</v>
+        <v>4.5115418623013399</v>
       </c>
       <c r="L8" s="9">
         <f t="shared" si="0"/>
-        <v>85.465647636764103</v>
-      </c>
-      <c r="O8" s="30" t="s">
-        <v>31</v>
+        <v>86.956808148753694</v>
+      </c>
+      <c r="O8" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="P8" s="9">
         <f>AVERAGE(L13:L18)</f>
-        <v>57.431032460319706</v>
-      </c>
-    </row>
-    <row r="9" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="25" t="s">
-        <v>14</v>
+        <v>60.334607670794327</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="D9" s="9">
-        <v>62.687672379754503</v>
+        <v>50.553712395398797</v>
       </c>
       <c r="E9" s="9">
-        <v>55.9809679783775</v>
-      </c>
-      <c r="F9" s="39">
-        <v>82.968447209422294</v>
+        <v>74.284368466285997</v>
+      </c>
+      <c r="F9" s="48">
+        <v>74.622316617628201</v>
       </c>
       <c r="G9" s="9">
-        <v>52.313537495321597</v>
+        <v>71.019966600588802</v>
       </c>
       <c r="H9" s="9">
-        <v>67.590276895690096</v>
-      </c>
-      <c r="I9" s="10">
-        <v>75.041964051563198</v>
+        <v>75.447000426318297</v>
+      </c>
+      <c r="I9" s="37">
+        <v>75.674632955774698</v>
       </c>
       <c r="J9" s="9">
-        <v>66.097144335021497</v>
+        <v>70.266999576999197</v>
       </c>
       <c r="K9" s="9">
-        <v>10.5737839796421</v>
+        <v>8.9476588904403602</v>
       </c>
       <c r="L9" s="9">
         <f t="shared" si="0"/>
-        <v>82.968447209422294</v>
-      </c>
-      <c r="O9" s="32" t="s">
-        <v>32</v>
+        <v>75.674632955774698</v>
+      </c>
+      <c r="O9" s="31" t="s">
+        <v>28</v>
       </c>
       <c r="P9" s="13">
         <f>_xlfn.STDEV.P(L13:L18)</f>
-        <v>26.866380179469502</v>
-      </c>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C10" s="25" t="s">
-        <v>15</v>
+        <v>28.334447139025311</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C10" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="D10" s="9">
-        <v>72.379691433975793</v>
+        <v>70.766842096210695</v>
       </c>
       <c r="E10" s="9">
-        <v>84.129149045305297</v>
-      </c>
-      <c r="F10" s="39">
-        <v>84.434784225361994</v>
+        <v>83.671431510681103</v>
+      </c>
+      <c r="F10" s="38">
+        <v>86.842415329459101</v>
       </c>
       <c r="G10" s="9">
-        <v>62.448038006191602</v>
+        <v>71.4157976208881</v>
       </c>
       <c r="H10" s="9">
-        <v>59.407050301560503</v>
+        <v>71.472025509189294</v>
       </c>
       <c r="I10" s="10">
-        <v>82.389965034228993</v>
+        <v>81.962624906808202</v>
       </c>
       <c r="J10" s="9">
-        <v>74.198113007770701</v>
+        <v>77.688522828872706</v>
       </c>
       <c r="K10" s="9">
-        <v>10.4801189602937</v>
+        <v>6.7839305479916101</v>
       </c>
       <c r="L10" s="9">
         <f t="shared" si="0"/>
-        <v>84.434784225361994</v>
-      </c>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C11" s="25" t="s">
-        <v>16</v>
+        <v>86.842415329459101</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C11" s="24" t="s">
+        <v>13</v>
       </c>
       <c r="D11" s="9">
         <v>71.623865796829904</v>
@@ -1148,7 +1153,7 @@
       <c r="H11" s="9">
         <v>79.597327200778096</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I11" s="37">
         <v>86.2456998048754</v>
       </c>
       <c r="J11" s="9">
@@ -1162,14 +1167,14 @@
         <v>86.2456998048754</v>
       </c>
     </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="26" t="s">
-        <v>17</v>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C12" s="25" t="s">
+        <v>14</v>
       </c>
       <c r="D12" s="11">
         <v>85.706501158796698</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12" s="39">
         <v>89.5311803768993</v>
       </c>
       <c r="F12" s="11">
@@ -1184,53 +1189,53 @@
       <c r="I12" s="12">
         <v>87.094576668028907</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="32">
         <v>87.366558833414203</v>
       </c>
-      <c r="K12" s="34">
+      <c r="K12" s="49">
         <v>3.2241142865407801</v>
       </c>
-      <c r="L12" s="34">
+      <c r="L12" s="33">
         <f t="shared" si="0"/>
         <v>89.5311803768993</v>
       </c>
     </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C13" s="27" t="s">
-        <v>18</v>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C13" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="D13" s="9">
-        <v>0.38252950285306198</v>
+        <v>60.168481406952999</v>
       </c>
       <c r="E13" s="9">
-        <v>0.96982594303256897</v>
-      </c>
-      <c r="F13" s="39">
-        <v>64.127047354602098</v>
+        <v>76.978833995825994</v>
+      </c>
+      <c r="F13" s="48">
+        <v>71.632966896838198</v>
       </c>
       <c r="G13" s="9">
-        <v>32.313391544379201</v>
+        <v>58.769922014162503</v>
       </c>
       <c r="H13" s="9">
-        <v>47.986932729520397</v>
-      </c>
-      <c r="I13" s="10">
-        <v>61.2054137488823</v>
+        <v>73.518812099485302</v>
+      </c>
+      <c r="I13" s="37">
+        <v>81.548498617449795</v>
       </c>
       <c r="J13" s="9">
-        <v>34.497523470544898</v>
+        <v>70.4362525051191</v>
       </c>
       <c r="K13" s="9">
-        <v>26.086578273576599</v>
+        <v>8.6400711500808693</v>
       </c>
       <c r="L13" s="9">
         <f t="shared" si="0"/>
-        <v>64.127047354602098</v>
-      </c>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C14" s="25" t="s">
-        <v>19</v>
+        <v>81.548498617449795</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C14" s="24" t="s">
+        <v>15</v>
       </c>
       <c r="D14" s="9">
         <v>72.081701296921494</v>
@@ -1247,7 +1252,7 @@
       <c r="H14" s="9">
         <v>13.6397556718434</v>
       </c>
-      <c r="I14" s="38">
+      <c r="I14" s="37">
         <v>84.958475731106901</v>
       </c>
       <c r="J14" s="9">
@@ -1261,9 +1266,9 @@
         <v>84.958475731106901</v>
       </c>
     </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="25" t="s">
-        <v>20</v>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C15" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="D15" s="9">
         <v>6.7363168563854599</v>
@@ -1280,7 +1285,7 @@
       <c r="H15" s="9">
         <v>9.2332568617153594</v>
       </c>
-      <c r="I15" s="38">
+      <c r="I15" s="37">
         <v>77.043635108852499</v>
       </c>
       <c r="J15" s="9">
@@ -1294,9 +1299,9 @@
         <v>77.043635108852499</v>
       </c>
     </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="26" t="s">
-        <v>21</v>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C16" s="25" t="s">
+        <v>17</v>
       </c>
       <c r="D16" s="11">
         <v>0</v>
@@ -1313,23 +1318,23 @@
       <c r="H16" s="11">
         <v>0</v>
       </c>
-      <c r="I16" s="41">
+      <c r="I16" s="40">
         <v>6.0964636980814904</v>
       </c>
-      <c r="J16" s="35">
+      <c r="J16" s="34">
         <v>1.5358807119079201</v>
       </c>
-      <c r="K16" s="45">
+      <c r="K16" s="33">
         <v>2.3359628287429199</v>
       </c>
-      <c r="L16" s="37">
+      <c r="L16" s="36">
         <f t="shared" si="0"/>
         <v>6.0964636980814904</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C17" s="25" t="s">
-        <v>22</v>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C17" s="24" t="s">
+        <v>18</v>
       </c>
       <c r="D17" s="9">
         <v>0</v>
@@ -1346,13 +1351,13 @@
       <c r="H17" s="9">
         <v>23.603852789045501</v>
       </c>
-      <c r="I17" s="38">
+      <c r="I17" s="37">
         <v>72.073629243816796</v>
       </c>
       <c r="J17" s="9">
         <v>23.076994181242899</v>
       </c>
-      <c r="K17" s="37">
+      <c r="K17" s="36">
         <v>26.467395933395998</v>
       </c>
       <c r="L17" s="20">
@@ -1360,9 +1365,9 @@
         <v>72.073629243816796</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="28" t="s">
-        <v>23</v>
+    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="27" t="s">
+        <v>19</v>
       </c>
       <c r="D18" s="13">
         <v>0</v>
@@ -1370,7 +1375,7 @@
       <c r="E18" s="13">
         <v>0</v>
       </c>
-      <c r="F18" s="42">
+      <c r="F18" s="41">
         <v>40.286943625458498</v>
       </c>
       <c r="G18" s="13">
@@ -1382,7 +1387,7 @@
       <c r="I18" s="14">
         <v>23.716781628940002</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="28">
         <v>10.7479382048686</v>
       </c>
       <c r="K18" s="13">
@@ -1393,9 +1398,9 @@
         <v>40.286943625458498</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="9">
@@ -1426,10 +1431,10 @@
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="C20" s="25" t="s">
-        <v>24</v>
+      <c r="C20" s="24" t="s">
+        <v>20</v>
       </c>
       <c r="D20" s="9">
         <f>MAX(D5:D18)</f>
@@ -1459,8 +1464,8 @@
       <c r="K20" s="18"/>
       <c r="L20" s="18"/>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="28" t="s">
+    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="27" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="13">
@@ -1491,21 +1496,21 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="26" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7" t="s">
@@ -1527,14 +1532,14 @@
         <v>8</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L27" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C28" s="22" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C28" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="15"/>
@@ -1570,12 +1575,12 @@
         <f>K28-J28</f>
         <v>11.613705447130613</v>
       </c>
-      <c r="N28" s="47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C29" s="22" t="s">
+      <c r="N28" s="45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C29" s="24" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="15"/>
@@ -1599,7 +1604,7 @@
         <f t="shared" si="4"/>
         <v>27.747682317926596</v>
       </c>
-      <c r="J29" s="43">
+      <c r="J29" s="50">
         <f t="shared" ref="J29:J41" si="5">MIN(E29:I29)</f>
         <v>1.8955122410410041</v>
       </c>
@@ -1612,8 +1617,8 @@
         <v>28.797885115804498</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C30" s="22" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C30" s="24" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="15"/>
@@ -1645,128 +1650,128 @@
         <f t="shared" si="6"/>
         <v>12.762430960072095</v>
       </c>
-      <c r="L30" s="44">
+      <c r="L30" s="43">
         <f t="shared" si="7"/>
         <v>34.463017224282197</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C31" s="22" t="s">
-        <v>13</v>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C31" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="9">
         <f t="shared" si="4"/>
-        <v>3.728728961536504</v>
+        <v>10.116669680787396</v>
       </c>
       <c r="F31" s="9">
         <f t="shared" si="4"/>
-        <v>6.8912763428899098</v>
+        <v>9.8983982157830894</v>
       </c>
       <c r="G31" s="9">
         <f t="shared" si="4"/>
-        <v>-17.250417272935593</v>
+        <v>2.7873295905880866</v>
       </c>
       <c r="H31" s="9">
         <f t="shared" si="4"/>
-        <v>-30.644229128951096</v>
+        <v>11.033321077061288</v>
       </c>
       <c r="I31" s="10">
         <f t="shared" si="4"/>
-        <v>5.9636693245820993</v>
+        <v>9.6228962847299897</v>
       </c>
       <c r="J31" s="9">
         <f t="shared" si="5"/>
-        <v>-30.644229128951096</v>
+        <v>2.7873295905880866</v>
       </c>
       <c r="K31" s="9">
         <f t="shared" si="6"/>
-        <v>6.8912763428899098</v>
-      </c>
-      <c r="L31" s="44">
+        <v>11.033321077061288</v>
+      </c>
+      <c r="L31" s="50">
         <f t="shared" si="7"/>
-        <v>37.535505471841006</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C32" s="22" t="s">
-        <v>14</v>
+        <v>8.2459914864732013</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C32" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="9">
         <f t="shared" si="4"/>
-        <v>-6.706704401377003</v>
+        <v>23.7306560708872</v>
       </c>
       <c r="F32" s="9">
         <f t="shared" si="4"/>
-        <v>20.280774829667791</v>
+        <v>24.068604222229403</v>
       </c>
       <c r="G32" s="9">
         <f t="shared" si="4"/>
-        <v>-10.374134884432905</v>
+        <v>20.466254205190005</v>
       </c>
       <c r="H32" s="9">
         <f t="shared" si="4"/>
-        <v>4.9026045159355931</v>
+        <v>24.8932880309195</v>
       </c>
       <c r="I32" s="10">
         <f t="shared" si="4"/>
-        <v>12.354291671808696</v>
-      </c>
-      <c r="J32" s="9">
+        <v>25.1209205603759</v>
+      </c>
+      <c r="J32" s="42">
         <f t="shared" si="5"/>
-        <v>-10.374134884432905</v>
+        <v>20.466254205190005</v>
       </c>
       <c r="K32" s="9">
         <f t="shared" si="6"/>
-        <v>20.280774829667791</v>
-      </c>
-      <c r="L32" s="44">
+        <v>25.1209205603759</v>
+      </c>
+      <c r="L32" s="50">
         <f t="shared" si="7"/>
-        <v>30.654909714100697</v>
-      </c>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="22" t="s">
-        <v>15</v>
+        <v>4.6546663551858956</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C33" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="9">
         <f t="shared" si="4"/>
-        <v>11.749457611329504</v>
+        <v>12.904589414470408</v>
       </c>
       <c r="F33" s="9">
         <f t="shared" si="4"/>
-        <v>12.055092791386201</v>
+        <v>16.075573233248406</v>
       </c>
       <c r="G33" s="9">
         <f t="shared" si="4"/>
-        <v>-9.931653427784191</v>
+        <v>0.64895552467740458</v>
       </c>
       <c r="H33" s="9">
         <f t="shared" si="4"/>
-        <v>-12.972641132415291</v>
+        <v>0.70518341297859877</v>
       </c>
       <c r="I33" s="10">
         <f t="shared" si="4"/>
-        <v>10.0102736002532</v>
+        <v>11.195782810597507</v>
       </c>
       <c r="J33" s="9">
         <f t="shared" si="5"/>
-        <v>-12.972641132415291</v>
+        <v>0.64895552467740458</v>
       </c>
       <c r="K33" s="9">
         <f t="shared" si="6"/>
-        <v>12.055092791386201</v>
+        <v>16.075573233248406</v>
       </c>
       <c r="L33" s="9">
         <f t="shared" si="7"/>
-        <v>25.027733923801492</v>
-      </c>
-    </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="22" t="s">
-        <v>16</v>
+        <v>15.426617708571001</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C34" s="24" t="s">
+        <v>13</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="9">
@@ -1802,9 +1807,9 @@
         <v>15.489887801922706</v>
       </c>
     </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C35" s="23" t="s">
-        <v>17</v>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C35" s="25" t="s">
+        <v>14</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="11">
@@ -1831,7 +1836,7 @@
         <f t="shared" si="5"/>
         <v>-2.2646861768049007</v>
       </c>
-      <c r="K35" s="36">
+      <c r="K35" s="35">
         <f t="shared" si="6"/>
         <v>3.8246792181026024</v>
       </c>
@@ -1840,47 +1845,47 @@
         <v>6.0893653949075031</v>
       </c>
     </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C36" s="22" t="s">
-        <v>18</v>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="9">
         <f t="shared" si="4"/>
-        <v>0.587296440179507</v>
+        <v>16.810352588872995</v>
       </c>
       <c r="F36" s="9">
         <f t="shared" si="4"/>
-        <v>63.744517851749038</v>
+        <v>11.464485489885199</v>
       </c>
       <c r="G36" s="9">
         <f t="shared" si="4"/>
-        <v>31.93086204152614</v>
+        <v>-1.3985593927904958</v>
       </c>
       <c r="H36" s="9">
         <f t="shared" si="4"/>
-        <v>47.604403226667337</v>
+        <v>13.350330692532303</v>
       </c>
       <c r="I36" s="10">
         <f t="shared" si="4"/>
-        <v>60.82288424602924</v>
+        <v>21.380017210496796</v>
       </c>
       <c r="J36" s="9">
         <f t="shared" si="5"/>
-        <v>0.587296440179507</v>
+        <v>-1.3985593927904958</v>
       </c>
       <c r="K36" s="9">
         <f t="shared" si="6"/>
-        <v>63.744517851749038</v>
-      </c>
-      <c r="L36" s="44">
+        <v>21.380017210496796</v>
+      </c>
+      <c r="L36" s="50">
         <f t="shared" si="7"/>
-        <v>63.15722141156953</v>
-      </c>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C37" s="22" t="s">
-        <v>19</v>
+        <v>22.778576603287291</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="24" t="s">
+        <v>15</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="9">
@@ -1903,7 +1908,7 @@
         <f t="shared" si="4"/>
         <v>12.876774434185407</v>
       </c>
-      <c r="J37" s="37">
+      <c r="J37" s="36">
         <f t="shared" si="5"/>
         <v>-58.441945625078091</v>
       </c>
@@ -1911,14 +1916,14 @@
         <f t="shared" si="6"/>
         <v>12.876774434185407</v>
       </c>
-      <c r="L37" s="44">
+      <c r="L37" s="43">
         <f t="shared" si="7"/>
         <v>71.318720059263498</v>
       </c>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="22" t="s">
-        <v>20</v>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C38" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="9">
@@ -1949,14 +1954,14 @@
         <f t="shared" si="6"/>
         <v>70.307318252467041</v>
       </c>
-      <c r="L38" s="44">
+      <c r="L38" s="43">
         <f t="shared" si="7"/>
         <v>73.869533847794727</v>
       </c>
     </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="23" t="s">
-        <v>21</v>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C39" s="25" t="s">
+        <v>17</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="11">
@@ -1992,9 +1997,9 @@
         <v>6.0964636980814904</v>
       </c>
     </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C40" s="22" t="s">
-        <v>22</v>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C40" s="24" t="s">
+        <v>18</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="9">
@@ -2021,18 +2026,18 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K40" s="43">
+      <c r="K40" s="42">
         <f t="shared" si="6"/>
         <v>72.073629243816796</v>
       </c>
-      <c r="L40" s="44">
+      <c r="L40" s="43">
         <f t="shared" si="7"/>
         <v>72.073629243816796</v>
       </c>
     </row>
-    <row r="41" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="24" t="s">
-        <v>23</v>
+    <row r="41" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C41" s="27" t="s">
+        <v>19</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="13">
@@ -2063,19 +2068,19 @@
         <f t="shared" si="6"/>
         <v>40.286943625458498</v>
       </c>
-      <c r="L41" s="46">
+      <c r="L41" s="44">
         <f t="shared" si="7"/>
         <v>40.286943625458498</v>
       </c>
     </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C42" s="22" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="9">
         <f>MIN(E28:E41)</f>
-        <v>-6.706704401377003</v>
+        <v>-3.5622155953276797</v>
       </c>
       <c r="F42" s="9">
         <f t="shared" ref="F42:I42" si="8">MIN(F28:F41)</f>
@@ -2083,7 +2088,7 @@
       </c>
       <c r="G42" s="9">
         <f t="shared" si="8"/>
-        <v>-17.250417272935593</v>
+        <v>-11.234232033118495</v>
       </c>
       <c r="H42" s="9">
         <f t="shared" si="8"/>
@@ -2097,14 +2102,14 @@
       <c r="K42" s="9"/>
       <c r="L42" s="9"/>
     </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C43" s="22" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="9">
         <f>MAX(E28:E41)</f>
-        <v>17.843195547852908</v>
+        <v>23.7306560708872</v>
       </c>
       <c r="F43" s="9">
         <f t="shared" ref="F43:I43" si="9">MAX(F28:F41)</f>
@@ -2116,7 +2121,7 @@
       </c>
       <c r="H43" s="9">
         <f t="shared" si="9"/>
-        <v>47.604403226667337</v>
+        <v>24.8932880309195</v>
       </c>
       <c r="I43" s="10">
         <f t="shared" si="9"/>
@@ -2126,14 +2131,14 @@
       <c r="K43" s="9"/>
       <c r="L43" s="9"/>
     </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C44" s="22" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="9">
         <f>E43-E42</f>
-        <v>24.549899949229911</v>
+        <v>27.292871666214879</v>
       </c>
       <c r="F44" s="9">
         <f t="shared" ref="F44:I44" si="10">F43-F42</f>
@@ -2141,11 +2146,11 @@
       </c>
       <c r="G44" s="9">
         <f t="shared" si="10"/>
-        <v>57.567589860220494</v>
+        <v>51.551404620403396</v>
       </c>
       <c r="H44" s="9">
         <f t="shared" si="10"/>
-        <v>106.04634885174542</v>
+        <v>83.335233655997598</v>
       </c>
       <c r="I44" s="10">
         <f t="shared" si="10"/>
@@ -2155,59 +2160,59 @@
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
     </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C45" s="22" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="9">
         <f>AVERAGE(E28:E41)</f>
-        <v>3.9633077090621174</v>
+        <v>7.8349855050156512</v>
       </c>
       <c r="F45" s="9">
         <f t="shared" ref="F45:I45" si="11">AVERAGE(F28:F41)</f>
-        <v>20.598470392428911</v>
+        <v>17.63671320281842</v>
       </c>
       <c r="G45" s="9">
         <f t="shared" si="11"/>
-        <v>3.8189977185448036</v>
+        <v>5.8282351093513425</v>
       </c>
       <c r="H45" s="9">
         <f t="shared" si="11"/>
-        <v>-0.70338907623556701</v>
+        <v>2.231752761782658</v>
       </c>
       <c r="I45" s="10">
         <f t="shared" si="11"/>
-        <v>24.298739949660707</v>
+        <v>22.739346951341201</v>
       </c>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
     </row>
-    <row r="46" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="24" t="s">
+    <row r="46" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C46" s="23" t="s">
         <v>7</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="13">
         <f>_xlfn.STDEV.P(E28:E41)</f>
-        <v>6.4454237951365903</v>
+        <v>7.8350386209437657</v>
       </c>
       <c r="F46" s="13">
         <f t="shared" ref="F46:I46" si="12">_xlfn.STDEV.P(F28:F41)</f>
-        <v>21.035217641671611</v>
+        <v>17.278760907683164</v>
       </c>
       <c r="G46" s="13">
         <f t="shared" si="12"/>
-        <v>16.971961154672947</v>
+        <v>13.801891695271944</v>
       </c>
       <c r="H46" s="13">
         <f t="shared" si="12"/>
-        <v>24.676996356919908</v>
+        <v>20.676280806402293</v>
       </c>
       <c r="I46" s="14">
         <f t="shared" si="12"/>
-        <v>23.69850447004832</v>
+        <v>21.057520638332274</v>
       </c>
       <c r="J46" s="13"/>
       <c r="K46" s="13"/>

</xml_diff>